<commit_message>
Cleaned up our tests
</commit_message>
<xml_diff>
--- a/Board_Layout_With_Color.xlsx
+++ b/Board_Layout_With_Color.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mason\Documents\School\Spring\Software Engineering\Clue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\eclipse-workspace\Clue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50752B21-E265-44DE-B2DF-3E5D18C6B3A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
   </bookViews>
   <sheets>
     <sheet name="Board_Layout" sheetId="1" r:id="rId1"/>
@@ -96,7 +95,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -452,16 +451,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF10" sqref="AF10"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -537,9 +536,11 @@
       <c r="Y1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Z1" s="1"/>
+      <c r="Z1" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -615,9 +616,11 @@
       <c r="Y2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Z2" s="1"/>
+      <c r="Z2" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -693,9 +696,11 @@
       <c r="Y3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Z3" s="1"/>
+      <c r="Z3" s="1">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -771,9 +776,11 @@
       <c r="Y4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Z4" s="1"/>
+      <c r="Z4" s="1">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -849,9 +856,11 @@
       <c r="Y5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Z5" s="1"/>
+      <c r="Z5" s="1">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -927,9 +936,11 @@
       <c r="Y6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Z6" s="1"/>
+      <c r="Z6" s="1">
+        <v>5</v>
+      </c>
     </row>
-    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -1005,9 +1016,11 @@
       <c r="Y7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Z7" s="1"/>
+      <c r="Z7" s="1">
+        <v>6</v>
+      </c>
     </row>
-    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
@@ -1083,9 +1096,11 @@
       <c r="Y8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Z8" s="1"/>
+      <c r="Z8" s="1">
+        <v>7</v>
+      </c>
     </row>
-    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1161,9 +1176,11 @@
       <c r="Y9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Z9" s="1"/>
+      <c r="Z9" s="1">
+        <v>8</v>
+      </c>
     </row>
-    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
@@ -1239,9 +1256,11 @@
       <c r="Y10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Z10" s="1"/>
+      <c r="Z10" s="1">
+        <v>9</v>
+      </c>
     </row>
-    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
@@ -1317,9 +1336,11 @@
       <c r="Y11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="Z11" s="1"/>
+      <c r="Z11" s="1">
+        <v>10</v>
+      </c>
     </row>
-    <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>2</v>
       </c>
@@ -1395,9 +1416,11 @@
       <c r="Y12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="Z12" s="1"/>
+      <c r="Z12" s="1">
+        <v>11</v>
+      </c>
     </row>
-    <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
@@ -1473,9 +1496,11 @@
       <c r="Y13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Z13" s="1"/>
+      <c r="Z13" s="1">
+        <v>12</v>
+      </c>
     </row>
-    <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
@@ -1551,9 +1576,11 @@
       <c r="Y14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Z14" s="1"/>
+      <c r="Z14" s="1">
+        <v>13</v>
+      </c>
     </row>
-    <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
@@ -1629,9 +1656,11 @@
       <c r="Y15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Z15" s="1"/>
+      <c r="Z15" s="1">
+        <v>14</v>
+      </c>
     </row>
-    <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -1707,9 +1736,11 @@
       <c r="Y16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Z16" s="1"/>
+      <c r="Z16" s="1">
+        <v>15</v>
+      </c>
     </row>
-    <row r="17" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -1785,9 +1816,11 @@
       <c r="Y17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Z17" s="1"/>
+      <c r="Z17" s="1">
+        <v>16</v>
+      </c>
     </row>
-    <row r="18" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -1863,9 +1896,11 @@
       <c r="Y18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Z18" s="1"/>
+      <c r="Z18" s="1">
+        <v>17</v>
+      </c>
     </row>
-    <row r="19" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -1941,9 +1976,11 @@
       <c r="Y19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Z19" s="1"/>
+      <c r="Z19" s="1">
+        <v>18</v>
+      </c>
     </row>
-    <row r="20" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
@@ -2019,9 +2056,11 @@
       <c r="Y20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Z20" s="1"/>
+      <c r="Z20" s="1">
+        <v>19</v>
+      </c>
     </row>
-    <row r="21" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
@@ -2097,9 +2136,11 @@
       <c r="Y21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Z21" s="1"/>
+      <c r="Z21" s="1">
+        <v>20</v>
+      </c>
     </row>
-    <row r="22" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>17</v>
       </c>
@@ -2175,9 +2216,11 @@
       <c r="Y22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Z22" s="1"/>
+      <c r="Z22" s="1">
+        <v>21</v>
+      </c>
     </row>
-    <row r="23" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>17</v>
       </c>
@@ -2253,9 +2296,11 @@
       <c r="Y23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Z23" s="1"/>
+      <c r="Z23" s="1">
+        <v>22</v>
+      </c>
     </row>
-    <row r="24" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>2</v>
       </c>
@@ -2331,9 +2376,11 @@
       <c r="Y24" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Z24" s="1"/>
+      <c r="Z24" s="1">
+        <v>23</v>
+      </c>
     </row>
-    <row r="25" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>2</v>
       </c>
@@ -2409,34 +2456,86 @@
       <c r="Y25" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Z25" s="1"/>
+      <c r="Z25" s="1">
+        <v>24</v>
+      </c>
     </row>
-    <row r="26" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
-      <c r="T26" s="1"/>
-      <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
-      <c r="W26" s="1"/>
-      <c r="X26" s="1"/>
-      <c r="Y26" s="1"/>
+    <row r="26" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>3</v>
+      </c>
+      <c r="E26" s="1">
+        <v>4</v>
+      </c>
+      <c r="F26" s="1">
+        <v>5</v>
+      </c>
+      <c r="G26" s="1">
+        <v>6</v>
+      </c>
+      <c r="H26" s="1">
+        <v>7</v>
+      </c>
+      <c r="I26" s="1">
+        <v>8</v>
+      </c>
+      <c r="J26" s="1">
+        <v>9</v>
+      </c>
+      <c r="K26" s="1">
+        <v>10</v>
+      </c>
+      <c r="L26" s="1">
+        <v>11</v>
+      </c>
+      <c r="M26" s="1">
+        <v>12</v>
+      </c>
+      <c r="N26" s="1">
+        <v>13</v>
+      </c>
+      <c r="O26" s="1">
+        <v>14</v>
+      </c>
+      <c r="P26" s="1">
+        <v>15</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>16</v>
+      </c>
+      <c r="R26" s="1">
+        <v>17</v>
+      </c>
+      <c r="S26" s="1">
+        <v>18</v>
+      </c>
+      <c r="T26" s="1">
+        <v>19</v>
+      </c>
+      <c r="U26" s="1">
+        <v>20</v>
+      </c>
+      <c r="V26" s="1">
+        <v>21</v>
+      </c>
+      <c r="W26" s="1">
+        <v>22</v>
+      </c>
+      <c r="X26" s="1">
+        <v>23</v>
+      </c>
+      <c r="Y26" s="1">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added colors to the spreadsheet to correspond to the tests
</commit_message>
<xml_diff>
--- a/Board_Layout_With_Color.xlsx
+++ b/Board_Layout_With_Color.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="23">
   <si>
     <t>L</t>
   </si>
@@ -91,6 +91,9 @@
   <si>
     <t>RU</t>
   </si>
+  <si>
+    <t>(10,24) is also light blue</t>
+  </si>
 </sst>
 </file>
 
@@ -113,7 +116,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,6 +147,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE3B5D7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -157,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -172,12 +211,33 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE3B5D7"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -452,16 +512,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z26"/>
+  <dimension ref="A1:AL28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -482,7 +542,7 @@
       <c r="G1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="4" t="s">
@@ -521,7 +581,7 @@
       <c r="T1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="11" t="s">
         <v>2</v>
       </c>
       <c r="V1" s="3" t="s">
@@ -540,7 +600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -620,7 +680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -700,7 +760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -780,7 +840,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -860,7 +920,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -940,7 +1000,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -989,7 +1049,7 @@
       <c r="P7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Q7" s="3" t="s">
+      <c r="Q7" s="6" t="s">
         <v>5</v>
       </c>
       <c r="R7" s="3" t="s">
@@ -1020,8 +1080,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1069,7 +1129,7 @@
       <c r="P8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="Q8" s="8" t="s">
         <v>10</v>
       </c>
       <c r="R8" s="3" t="s">
@@ -1100,14 +1160,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -1164,7 +1224,7 @@
       <c r="U9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="V9" s="4" t="s">
+      <c r="V9" s="9" t="s">
         <v>2</v>
       </c>
       <c r="W9" s="2" t="s">
@@ -1180,14 +1240,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -1260,11 +1320,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1306,13 +1366,13 @@
       <c r="O11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="P11" s="3" t="s">
+      <c r="P11" s="6" t="s">
         <v>11</v>
       </c>
       <c r="Q11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R11" s="2" t="s">
+      <c r="R11" s="8" t="s">
         <v>13</v>
       </c>
       <c r="S11" s="3" t="s">
@@ -1333,14 +1393,14 @@
       <c r="X11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="Y11" s="4" t="s">
+      <c r="Y11" s="10" t="s">
         <v>2</v>
       </c>
       <c r="Z11" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>2</v>
       </c>
@@ -1353,7 +1413,7 @@
       <c r="D12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="10" t="s">
         <v>2</v>
       </c>
       <c r="F12" s="4" t="s">
@@ -1413,14 +1473,14 @@
       <c r="X12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="Y12" s="4" t="s">
+      <c r="Y12" s="11" t="s">
         <v>2</v>
       </c>
       <c r="Z12" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
@@ -1448,7 +1508,7 @@
       <c r="I13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J13" s="10" t="s">
         <v>2</v>
       </c>
       <c r="K13" s="4" t="s">
@@ -1484,10 +1544,10 @@
       <c r="U13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="V13" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="W13" s="2" t="s">
+      <c r="V13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="W13" s="8" t="s">
         <v>16</v>
       </c>
       <c r="X13" s="2" t="s">
@@ -1500,8 +1560,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1580,7 +1640,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
@@ -1632,7 +1692,7 @@
       <c r="Q15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R15" s="3" t="s">
+      <c r="R15" s="6" t="s">
         <v>11</v>
       </c>
       <c r="S15" s="3" t="s">
@@ -1659,8 +1719,9 @@
       <c r="Z15" s="1">
         <v>14</v>
       </c>
+      <c r="AL15" s="7"/>
     </row>
-    <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -1771,7 +1832,7 @@
       <c r="J17" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="9" t="s">
         <v>2</v>
       </c>
       <c r="L17" s="4" t="s">
@@ -1860,7 +1921,7 @@
       <c r="M18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="N18" s="4" t="s">
+      <c r="N18" s="11" t="s">
         <v>2</v>
       </c>
       <c r="O18" s="4" t="s">
@@ -1999,13 +2060,13 @@
       <c r="F20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I20" s="4" t="s">
+      <c r="H20" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I20" s="11" t="s">
         <v>2</v>
       </c>
       <c r="J20" s="3" t="s">
@@ -2278,7 +2339,7 @@
       <c r="S23" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="T23" s="2" t="s">
+      <c r="T23" s="8" t="s">
         <v>15</v>
       </c>
       <c r="U23" s="3" t="s">
@@ -2381,7 +2442,7 @@
       </c>
     </row>
     <row r="25" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -2432,10 +2493,10 @@
       <c r="Q25" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="R25" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="S25" s="4" t="s">
+      <c r="R25" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="S25" s="10" t="s">
         <v>2</v>
       </c>
       <c r="T25" s="3" t="s">
@@ -2535,6 +2596,11 @@
       </c>
       <c r="Y26" s="1">
         <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added text describing the colors in the spreadsheet
</commit_message>
<xml_diff>
--- a/Board_Layout_With_Color.xlsx
+++ b/Board_Layout_With_Color.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="30">
   <si>
     <t>L</t>
   </si>
@@ -93,6 +93,27 @@
   </si>
   <si>
     <t>(10,24) is also light blue</t>
+  </si>
+  <si>
+    <t>Number of doors: 14</t>
+  </si>
+  <si>
+    <t>White: Door direction tests (in BoardInitTests)</t>
+  </si>
+  <si>
+    <t>Orange: adjacency list tests, inside room</t>
+  </si>
+  <si>
+    <t>Purple: adjacency list tests, room exits</t>
+  </si>
+  <si>
+    <t>Green: adjacency lists beside room entrance</t>
+  </si>
+  <si>
+    <t>Light Purple: walkway scenarios</t>
+  </si>
+  <si>
+    <t>Light Blue: test targets</t>
   </si>
 </sst>
 </file>
@@ -512,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL28"/>
+  <dimension ref="A1:AL35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2603,6 +2624,41 @@
         <v>22</v>
       </c>
     </row>
+    <row r="29" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Made some color description in the spreadsheet
</commit_message>
<xml_diff>
--- a/Board_Layout_With_Color.xlsx
+++ b/Board_Layout_With_Color.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="31">
   <si>
     <t>L</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Light Blue: test targets</t>
+  </si>
+  <si>
+    <t>(0,0) is also white</t>
   </si>
 </sst>
 </file>
@@ -217,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -246,6 +249,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -536,7 +542,7 @@
   <dimension ref="A1:AL35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -640,10 +646,10 @@
       <c r="F2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="12" t="s">
         <v>2</v>
       </c>
       <c r="I2" s="4" t="s">
@@ -1150,7 +1156,7 @@
       <c r="P8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Q8" s="8" t="s">
+      <c r="Q8" s="12" t="s">
         <v>10</v>
       </c>
       <c r="R8" s="3" t="s">
@@ -1248,7 +1254,7 @@
       <c r="V9" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="W9" s="2" t="s">
+      <c r="W9" s="12" t="s">
         <v>9</v>
       </c>
       <c r="X9" s="3" t="s">
@@ -1936,7 +1942,7 @@
       <c r="K18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="L18" s="12" t="s">
         <v>21</v>
       </c>
       <c r="M18" s="3" t="s">
@@ -2617,6 +2623,11 @@
       </c>
       <c r="Y26" s="1">
         <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>